<commit_message>
Add a chart showing the results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgewaters/Documents/Developer/Python/Monopoly-Probabilities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE0218E-CD70-6F42-A73D-1EA4A53A2612}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23588C2-E2FA-EE40-B384-E9DEE710A4E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="33580" windowHeight="19440" xr2:uid="{6C80073E-F3F0-0F45-928D-5DAAEF045DC2}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="33580" windowHeight="19440" activeTab="1" xr2:uid="{6C80073E-F3F0-0F45-928D-5DAAEF045DC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Chart1" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -166,9 +167,6 @@
     <t>1M</t>
   </si>
   <si>
-    <t>Probability     (Mine 1B)</t>
-  </si>
-  <si>
     <t>100T</t>
   </si>
   <si>
@@ -179,6 +177,9 @@
   </si>
   <si>
     <t>10B</t>
+  </si>
+  <si>
+    <t>Probability (Mine 1B)</t>
   </si>
 </sst>
 </file>
@@ -244,16 +245,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -262,6 +260,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -285,6 +289,1459 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800"/>
+              <a:t>Monopoly</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
+              <a:t> Probabilities</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Probability (Standupmaths)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$4:$B$44</c:f>
+              <c:strCache>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>Go</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mediterranean Avenue</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Community Chest</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Baltic Avenue</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Income Tax</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Reading Railroad</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Oriental Avenue</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Chance</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Vermont Avenue</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Connecticut Avenue</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Just Visiting Jail</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>St. Charles Place</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Electric Company</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>States Avenue</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Virginia Avenue</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Pennsylvania Railroad</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>St. James Place</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Community Chest</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Tennessee Avenue</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>New York Avenue</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Free Parking</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Kentucky Avenue</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Chance</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Indiana Avenue</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Illinois Avenue</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>B. &amp; O. Railroad</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Atlantic Avenue</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Ventnor Avenue</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Water Works</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Marvin Gardens</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Go To Jail</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Pacific Avenue</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>North Carolina Avenue</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Community Chest</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Pennsylvania Avenue</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Short Line Railroad</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Chance</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Park Place</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Luxury Tax</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Boardwalk</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>In Jail</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$C$44</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>2.8539999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1090000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9189999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2610000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4039999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.7570000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.317E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.017E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.308E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.2780000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.3250000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.7189999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.6100000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.3949999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.477E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.8039999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.6200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.9399999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.0960000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.8680000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.8389999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.2120000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.7310000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.1969999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.8969999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.7189999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.6890000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8209999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.6009999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.6749999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.6159999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.116E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.494E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.5530000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.239E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.085E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.086E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.5520000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F91F-094C-BA74-78BFF69B32FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Probability (Mine 1B)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$4:$B$44</c:f>
+              <c:strCache>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>Go</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mediterranean Avenue</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Community Chest</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Baltic Avenue</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Income Tax</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Reading Railroad</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Oriental Avenue</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Chance</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Vermont Avenue</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Connecticut Avenue</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Just Visiting Jail</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>St. Charles Place</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Electric Company</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>States Avenue</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Virginia Avenue</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Pennsylvania Railroad</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>St. James Place</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Community Chest</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Tennessee Avenue</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>New York Avenue</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Free Parking</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Kentucky Avenue</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Chance</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Indiana Avenue</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Illinois Avenue</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>B. &amp; O. Railroad</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Atlantic Avenue</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Ventnor Avenue</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Water Works</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Marvin Gardens</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Go To Jail</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Pacific Avenue</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>North Carolina Avenue</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Community Chest</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Pennsylvania Avenue</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Short Line Railroad</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Chance</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Park Place</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Luxury Tax</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Boardwalk</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>In Jail</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$44</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>3.0890000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1389999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8919999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.18E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.3439999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.828E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.273E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0109999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3220000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.299E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.2700000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.7009999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.6020000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.3800000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.4760000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.7900000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.801E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.605E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.9360000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.0810000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.869E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.8230000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.214E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.7220000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.1739999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.8879999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.7099999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.6839999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.811E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.5919999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.666E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.606E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.368E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.486E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.419E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.0059999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.179E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.179E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.6249999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.9600000000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F91F-094C-BA74-78BFF69B32FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1885112959"/>
+        <c:axId val="1885160383"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1885112959"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1885160383"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1885160383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1885112959"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{538EC0C1-DA5C-3042-8F30-8862B4EF49FE}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="154" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="5" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="11421753" cy="6275779"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40570D0D-8722-9841-B91D-ECAF3864E3A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -586,43 +2043,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD8CFF4-08F0-634F-9AEA-A4D4C775E343}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="46.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="18.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" style="2" customWidth="1"/>
     <col min="5" max="9" width="10.83203125" style="2"/>
     <col min="10" max="12" width="0" style="2" hidden="1" customWidth="1"/>
     <col min="13" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>44</v>
+      <c r="D2" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -643,7 +2102,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="10"/>
+      <c r="K4" s="9"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -669,7 +2128,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="10"/>
+      <c r="K5" s="9"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -695,7 +2154,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="10"/>
+      <c r="K6" s="9"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -721,7 +2180,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="10"/>
+      <c r="K7" s="9"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -747,7 +2206,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="10"/>
+      <c r="K8" s="9"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -773,7 +2232,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="10"/>
+      <c r="K9" s="9"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -799,7 +2258,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="10"/>
+      <c r="K10" s="9"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -825,7 +2284,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="10"/>
+      <c r="K11" s="9"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -851,7 +2310,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="10"/>
+      <c r="K12" s="9"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -877,7 +2336,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="10"/>
+      <c r="K13" s="9"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -903,7 +2362,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="10"/>
+      <c r="K14" s="9"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -929,7 +2388,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="10"/>
+      <c r="K15" s="9"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -955,7 +2414,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="10"/>
+      <c r="K16" s="9"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -981,7 +2440,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="10"/>
+      <c r="K17" s="9"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -1007,7 +2466,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="10"/>
+      <c r="K18" s="9"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -1033,7 +2492,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="10"/>
+      <c r="K19" s="9"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -1059,7 +2518,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="10"/>
+      <c r="K20" s="9"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -1085,7 +2544,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="10"/>
+      <c r="K21" s="9"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -1111,7 +2570,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="10"/>
+      <c r="K22" s="9"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -1137,7 +2596,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
-      <c r="K23" s="10"/>
+      <c r="K23" s="9"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -1163,7 +2622,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
-      <c r="K24" s="10"/>
+      <c r="K24" s="9"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -1189,7 +2648,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
-      <c r="K25" s="10"/>
+      <c r="K25" s="9"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -1215,7 +2674,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
-      <c r="K26" s="10"/>
+      <c r="K26" s="9"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -1241,7 +2700,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
-      <c r="K27" s="10"/>
+      <c r="K27" s="9"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
@@ -1267,7 +2726,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
-      <c r="K28" s="10"/>
+      <c r="K28" s="9"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
@@ -1293,7 +2752,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
-      <c r="K29" s="10"/>
+      <c r="K29" s="9"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
@@ -1319,7 +2778,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
-      <c r="K30" s="10"/>
+      <c r="K30" s="9"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
@@ -1345,7 +2804,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
-      <c r="K31" s="10"/>
+      <c r="K31" s="9"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
@@ -1371,7 +2830,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="10"/>
+      <c r="K32" s="9"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
@@ -1397,7 +2856,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="10"/>
+      <c r="K33" s="9"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
@@ -1423,7 +2882,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
-      <c r="K34" s="10"/>
+      <c r="K34" s="9"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
@@ -1449,7 +2908,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
-      <c r="K35" s="10"/>
+      <c r="K35" s="9"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
@@ -1475,7 +2934,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
-      <c r="K36" s="10"/>
+      <c r="K36" s="9"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
@@ -1501,7 +2960,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
-      <c r="K37" s="10"/>
+      <c r="K37" s="9"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
@@ -1527,7 +2986,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
-      <c r="K38" s="10"/>
+      <c r="K38" s="9"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
@@ -1553,13 +3012,13 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
-      <c r="K39" s="10"/>
+      <c r="K39" s="9"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1579,7 +3038,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
-      <c r="K40" s="10"/>
+      <c r="K40" s="9"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
@@ -1605,7 +3064,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
-      <c r="K41" s="10"/>
+      <c r="K41" s="9"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
@@ -1631,7 +3090,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
-      <c r="K42" s="10"/>
+      <c r="K42" s="9"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
@@ -1657,7 +3116,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
-      <c r="K43" s="10"/>
+      <c r="K43" s="9"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
@@ -1671,7 +3130,7 @@
       <c r="B44" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="8" t="s">
         <v>41</v>
       </c>
       <c r="D44" s="3">
@@ -1690,7 +3149,8 @@
       <c r="C45" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
+    <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
   </mergeCells>
@@ -1715,7 +3175,7 @@
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>43</v>
@@ -1724,13 +3184,13 @@
         <v>42</v>
       </c>
       <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
         <v>46</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>47</v>
-      </c>
-      <c r="F3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add results from the 10B turn sim
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgewaters/Documents/Developer/Python/Monopoly-Probabilities/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Monopoly-Probabilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23588C2-E2FA-EE40-B384-E9DEE710A4E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB6CD19-984D-4926-8EB2-8A0C040F6AB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="33580" windowHeight="19440" activeTab="1" xr2:uid="{6C80073E-F3F0-0F45-928D-5DAAEF045DC2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{6C80073E-F3F0-0F45-928D-5DAAEF045DC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Chart1" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Income Tax</t>
   </si>
@@ -179,13 +179,19 @@
     <t>10B</t>
   </si>
   <si>
-    <t>Probability (Mine 1B)</t>
+    <t>Probability (Mine 10B)</t>
+  </si>
+  <si>
+    <t>*This took 31 mins 12 seconds on Nebula</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -245,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -261,10 +267,17 @@
     </xf>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -674,7 +687,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Probability (Mine 1B)</c:v>
+                  <c:v>Probability (Mine 10B)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -827,7 +840,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>3.0890000000000001E-2</c:v>
+                  <c:v>3.09E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.1389999999999999E-2</c:v>
@@ -839,10 +852,10 @@
                   <c:v>2.18E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3439999999999999E-2</c:v>
+                  <c:v>2.3429999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.828E-2</c:v>
+                  <c:v>2.8289999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2.273E-2</c:v>
@@ -851,7 +864,7 @@
                   <c:v>1.0109999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.3220000000000001E-2</c:v>
+                  <c:v>2.3210000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2.299E-2</c:v>
@@ -887,7 +900,7 @@
                   <c:v>3.0810000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.869E-2</c:v>
+                  <c:v>2.87E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>2.8230000000000002E-2</c:v>
@@ -896,7 +909,7 @@
                   <c:v>1.214E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.7220000000000001E-2</c:v>
+                  <c:v>2.7210000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>3.1739999999999997E-2</c:v>
@@ -905,22 +918,22 @@
                   <c:v>2.8879999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.7099999999999999E-2</c:v>
+                  <c:v>2.7089999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>2.6839999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.811E-2</c:v>
+                  <c:v>2.8119999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.5919999999999999E-2</c:v>
+                  <c:v>2.5930000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.666E-2</c:v>
+                  <c:v>2.6669999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>2.606E-2</c:v>
@@ -929,10 +942,10 @@
                   <c:v>2.368E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.486E-2</c:v>
+                  <c:v>2.4850000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.419E-2</c:v>
+                  <c:v>2.418E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>1.0059999999999999E-2</c:v>
@@ -944,10 +957,10 @@
                   <c:v>2.179E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.6249999999999999E-2</c:v>
+                  <c:v>2.6259999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.9600000000000003E-2</c:v>
+                  <c:v>3.9609999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -996,7 +1009,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1703,10 +1716,10 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{538EC0C1-DA5C-3042-8F30-8862B4EF49FE}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="154" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="5" orientation="landscape"/>
   <drawing r:id="rId1"/>
 </chartsheet>
 </file>
@@ -1715,7 +1728,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="11421753" cy="6275779"/>
+    <xdr:ext cx="11405784" cy="6288114"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2044,46 +2057,46 @@
   <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="10.875" style="2"/>
     <col min="2" max="2" width="46.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="18.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" style="2" customWidth="1"/>
-    <col min="5" max="9" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="17.125" style="2" customWidth="1"/>
+    <col min="5" max="9" width="10.875" style="2"/>
     <col min="10" max="12" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="2"/>
+    <col min="13" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>0</v>
       </c>
@@ -2094,7 +2107,7 @@
         <v>2.8539999999999999E-2</v>
       </c>
       <c r="D4" s="3">
-        <v>3.0890000000000001E-2</v>
+        <v>3.09E-2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -2108,7 +2121,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <f>A4+1</f>
         <v>1</v>
@@ -2134,7 +2147,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A44" si="0">A5+1</f>
         <v>2</v>
@@ -2160,7 +2173,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2186,7 +2199,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2198,7 +2211,7 @@
         <v>2.4039999999999999E-2</v>
       </c>
       <c r="D8" s="3">
-        <v>2.3439999999999999E-2</v>
+        <v>2.3429999999999999E-2</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -2212,7 +2225,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2224,7 +2237,7 @@
         <v>2.7570000000000001E-2</v>
       </c>
       <c r="D9" s="3">
-        <v>2.828E-2</v>
+        <v>2.8289999999999999E-2</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -2238,7 +2251,7 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2264,7 +2277,7 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2290,7 +2303,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2302,7 +2315,7 @@
         <v>2.308E-2</v>
       </c>
       <c r="D12" s="3">
-        <v>2.3220000000000001E-2</v>
+        <v>2.3210000000000001E-2</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -2316,7 +2329,7 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2342,7 +2355,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2368,7 +2381,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2394,7 +2407,7 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2420,7 +2433,7 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2446,7 +2459,7 @@
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2472,7 +2485,7 @@
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2498,7 +2511,7 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2524,7 +2537,7 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2550,7 +2563,7 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2576,7 +2589,7 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2602,7 +2615,7 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2614,7 +2627,7 @@
         <v>2.8680000000000001E-2</v>
       </c>
       <c r="D24" s="3">
-        <v>2.869E-2</v>
+        <v>2.87E-2</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -2628,7 +2641,7 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2654,7 +2667,7 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2680,7 +2693,7 @@
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2692,7 +2705,7 @@
         <v>2.7310000000000001E-2</v>
       </c>
       <c r="D27" s="3">
-        <v>2.7220000000000001E-2</v>
+        <v>2.7210000000000002E-2</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -2706,7 +2719,7 @@
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2732,7 +2745,7 @@
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2758,7 +2771,7 @@
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2770,7 +2783,7 @@
         <v>2.7189999999999999E-2</v>
       </c>
       <c r="D30" s="3">
-        <v>2.7099999999999999E-2</v>
+        <v>2.7089999999999999E-2</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -2784,7 +2797,7 @@
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2810,7 +2823,7 @@
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2822,7 +2835,7 @@
         <v>2.8209999999999999E-2</v>
       </c>
       <c r="D32" s="3">
-        <v>2.811E-2</v>
+        <v>2.8119999999999999E-2</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2836,7 +2849,7 @@
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2848,7 +2861,7 @@
         <v>2.6009999999999998E-2</v>
       </c>
       <c r="D33" s="3">
-        <v>2.5919999999999999E-2</v>
+        <v>2.5930000000000002E-2</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2862,7 +2875,7 @@
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2888,7 +2901,7 @@
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2900,7 +2913,7 @@
         <v>2.6749999999999999E-2</v>
       </c>
       <c r="D35" s="3">
-        <v>2.666E-2</v>
+        <v>2.6669999999999999E-2</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2914,7 +2927,7 @@
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2940,7 +2953,7 @@
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -2966,7 +2979,7 @@
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2978,7 +2991,7 @@
         <v>2.494E-2</v>
       </c>
       <c r="D38" s="3">
-        <v>2.486E-2</v>
+        <v>2.4850000000000001E-2</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2992,7 +3005,7 @@
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -3004,7 +3017,7 @@
         <v>2.5530000000000001E-2</v>
       </c>
       <c r="D39" s="3">
-        <v>2.419E-2</v>
+        <v>2.418E-2</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -3018,7 +3031,7 @@
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
     </row>
-    <row r="40" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -3044,7 +3057,7 @@
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -3070,7 +3083,7 @@
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -3096,7 +3109,7 @@
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -3108,7 +3121,7 @@
         <v>2.5520000000000001E-2</v>
       </c>
       <c r="D43" s="3">
-        <v>2.6249999999999999E-2</v>
+        <v>2.6259999999999999E-2</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -3122,7 +3135,7 @@
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -3134,7 +3147,7 @@
         <v>41</v>
       </c>
       <c r="D44" s="3">
-        <v>3.9600000000000003E-2</v>
+        <v>3.9609999999999999E-2</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -3145,7 +3158,7 @@
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C45" s="3"/>
     </row>
   </sheetData>
@@ -3165,15 +3178,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD675E7-CB24-0F46-9876-B3D10253DD99}">
-  <dimension ref="A3:F46"/>
+  <dimension ref="A3:F52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -3193,7 +3206,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3.109E-2</v>
       </c>
@@ -3206,11 +3219,14 @@
       <c r="D4" s="1">
         <v>3.09E-2</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="12">
         <v>3.0890000000000001E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F4" s="12">
+        <v>3.09E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2.1100000000000001E-2</v>
       </c>
@@ -3223,11 +3239,14 @@
       <c r="D5" s="1">
         <v>2.1389999999999999E-2</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="12">
         <v>2.1389999999999999E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F5" s="12">
+        <v>2.1389999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1.8919999999999999E-2</v>
       </c>
@@ -3240,11 +3259,14 @@
       <c r="D6" s="1">
         <v>1.891E-2</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="12">
         <v>1.8919999999999999E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F6" s="12">
+        <v>1.8919999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2.0879999999999999E-2</v>
       </c>
@@ -3257,11 +3279,14 @@
       <c r="D7" s="1">
         <v>2.181E-2</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="12">
         <v>2.18E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F7" s="12">
+        <v>2.18E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2.401E-2</v>
       </c>
@@ -3274,11 +3299,14 @@
       <c r="D8" s="1">
         <v>2.3460000000000002E-2</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="12">
         <v>2.3439999999999999E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F8" s="12">
+        <v>2.3429999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2.9649999999999999E-2</v>
       </c>
@@ -3291,11 +3319,14 @@
       <c r="D9" s="1">
         <v>2.8289999999999999E-2</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="12">
         <v>2.8289999999999999E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F9" s="12">
+        <v>2.8289999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2.24E-2</v>
       </c>
@@ -3308,11 +3339,14 @@
       <c r="D10" s="1">
         <v>2.2710000000000001E-2</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="12">
         <v>2.273E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F10" s="12">
+        <v>2.273E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9.8499999999999994E-3</v>
       </c>
@@ -3325,11 +3359,14 @@
       <c r="D11" s="1">
         <v>1.013E-2</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="12">
         <v>1.0120000000000001E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F11" s="12">
+        <v>1.0109999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2.2530000000000001E-2</v>
       </c>
@@ -3342,11 +3379,14 @@
       <c r="D12" s="1">
         <v>2.3220000000000001E-2</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="12">
         <v>2.3210000000000001E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F12" s="12">
+        <v>2.3210000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2.3359999999999999E-2</v>
       </c>
@@ -3359,11 +3399,14 @@
       <c r="D13" s="1">
         <v>2.3009999999999999E-2</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="12">
         <v>2.299E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F13" s="12">
+        <v>2.299E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2.29E-2</v>
       </c>
@@ -3376,11 +3419,14 @@
       <c r="D14" s="1">
         <v>2.2700000000000001E-2</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="12">
         <v>2.2700000000000001E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F14" s="12">
+        <v>2.2700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2.726E-2</v>
       </c>
@@ -3393,11 +3439,14 @@
       <c r="D15" s="1">
         <v>2.6970000000000001E-2</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="12">
         <v>2.7E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F15" s="12">
+        <v>2.7009999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2.596E-2</v>
       </c>
@@ -3410,11 +3459,14 @@
       <c r="D16" s="1">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="12">
         <v>2.6020000000000001E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="12">
+        <v>2.6020000000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2.29E-2</v>
       </c>
@@ -3427,11 +3479,14 @@
       <c r="D17" s="1">
         <v>2.383E-2</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="12">
         <v>2.3800000000000002E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="12">
+        <v>2.3800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2.5010000000000001E-2</v>
       </c>
@@ -3444,11 +3499,14 @@
       <c r="D18" s="1">
         <v>2.477E-2</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="12">
         <v>2.4760000000000001E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="12">
+        <v>2.4760000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2.8039999999999999E-2</v>
       </c>
@@ -3461,11 +3519,14 @@
       <c r="D19" s="1">
         <v>2.792E-2</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="12">
         <v>2.7900000000000001E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="12">
+        <v>2.7900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2.726E-2</v>
       </c>
@@ -3478,11 +3539,14 @@
       <c r="D20" s="1">
         <v>2.7990000000000001E-2</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="12">
         <v>2.802E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="12">
+        <v>2.801E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2.6089999999999999E-2</v>
       </c>
@@ -3495,11 +3559,14 @@
       <c r="D21" s="1">
         <v>2.6040000000000001E-2</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="12">
         <v>2.6040000000000001E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="12">
+        <v>2.605E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2.9149999999999999E-2</v>
       </c>
@@ -3512,11 +3579,14 @@
       <c r="D22" s="1">
         <v>2.9340000000000001E-2</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="12">
         <v>2.9360000000000001E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="12">
+        <v>2.9360000000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>3.1E-2</v>
       </c>
@@ -3529,11 +3599,14 @@
       <c r="D23" s="1">
         <v>3.082E-2</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="12">
         <v>3.0810000000000001E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="12">
+        <v>3.0810000000000001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2.9350000000000001E-2</v>
       </c>
@@ -3546,11 +3619,14 @@
       <c r="D24" s="1">
         <v>2.87E-2</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="12">
         <v>2.87E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="12">
+        <v>2.87E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2.844E-2</v>
       </c>
@@ -3563,11 +3639,14 @@
       <c r="D25" s="1">
         <v>2.8230000000000002E-2</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="12">
         <v>2.8230000000000002E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="12">
+        <v>2.8230000000000002E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1.2120000000000001E-2</v>
       </c>
@@ -3580,11 +3659,14 @@
       <c r="D26" s="1">
         <v>1.2149999999999999E-2</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="12">
         <v>1.214E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="12">
+        <v>1.214E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2.6800000000000001E-2</v>
       </c>
@@ -3597,11 +3679,14 @@
       <c r="D27" s="1">
         <v>2.7199999999999998E-2</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="12">
         <v>2.7210000000000002E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="12">
+        <v>2.7210000000000002E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>3.2009999999999997E-2</v>
       </c>
@@ -3614,11 +3699,14 @@
       <c r="D28" s="1">
         <v>3.1759999999999997E-2</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="12">
         <v>3.175E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="12">
+        <v>3.1739999999999997E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2.8299999999999999E-2</v>
       </c>
@@ -3631,11 +3719,14 @@
       <c r="D29" s="1">
         <v>2.887E-2</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="12">
         <v>2.887E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="12">
+        <v>2.8879999999999999E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2.665E-2</v>
       </c>
@@ -3648,11 +3739,14 @@
       <c r="D30" s="1">
         <v>2.7089999999999999E-2</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="12">
         <v>2.7089999999999999E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="12">
+        <v>2.7089999999999999E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2.7089999999999999E-2</v>
       </c>
@@ -3665,11 +3759,14 @@
       <c r="D31" s="1">
         <v>2.6859999999999998E-2</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31" s="12">
         <v>2.6839999999999999E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="12">
+        <v>2.6839999999999999E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2.8920000000000001E-2</v>
       </c>
@@ -3682,11 +3779,14 @@
       <c r="D32" s="1">
         <v>2.81E-2</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" s="12">
         <v>2.8119999999999999E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="12">
+        <v>2.8119999999999999E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2.6069999999999999E-2</v>
       </c>
@@ -3699,11 +3799,14 @@
       <c r="D33" s="1">
         <v>2.5919999999999999E-2</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33" s="12">
         <v>2.5930000000000002E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="12">
+        <v>2.5930000000000002E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>0</v>
       </c>
@@ -3716,11 +3819,14 @@
       <c r="D34" s="1">
         <v>0</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2.6870000000000002E-2</v>
       </c>
@@ -3733,11 +3839,14 @@
       <c r="D35" s="1">
         <v>2.6679999999999999E-2</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="12">
         <v>2.6679999999999999E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="12">
+        <v>2.6669999999999999E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2.615E-2</v>
       </c>
@@ -3750,11 +3859,14 @@
       <c r="D36" s="1">
         <v>2.606E-2</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36" s="12">
         <v>2.606E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="12">
+        <v>2.606E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2.3429999999999999E-2</v>
       </c>
@@ -3767,11 +3879,14 @@
       <c r="D37" s="1">
         <v>2.3689999999999999E-2</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" s="12">
         <v>2.368E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="12">
+        <v>2.368E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2.469E-2</v>
       </c>
@@ -3784,11 +3899,14 @@
       <c r="D38" s="1">
         <v>2.4879999999999999E-2</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="12">
         <v>2.4850000000000001E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="12">
+        <v>2.4850000000000001E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2.4580000000000001E-2</v>
       </c>
@@ -3801,11 +3919,14 @@
       <c r="D39" s="1">
         <v>2.418E-2</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="12">
         <v>2.4170000000000001E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="12">
+        <v>2.418E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>1.001E-2</v>
       </c>
@@ -3818,11 +3939,14 @@
       <c r="D40" s="1">
         <v>1.005E-2</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="12">
         <v>1.0059999999999999E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="12">
+        <v>1.0059999999999999E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2.2079999999999999E-2</v>
       </c>
@@ -3835,11 +3959,14 @@
       <c r="D41" s="1">
         <v>2.1780000000000001E-2</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41" s="12">
         <v>2.179E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" s="12">
+        <v>2.179E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2.145E-2</v>
       </c>
@@ -3852,11 +3979,14 @@
       <c r="D42" s="1">
         <v>2.1760000000000002E-2</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E42" s="12">
         <v>2.179E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" s="12">
+        <v>2.179E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2.6089999999999999E-2</v>
       </c>
@@ -3869,11 +3999,14 @@
       <c r="D43" s="1">
         <v>2.6270000000000002E-2</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E43" s="12">
         <v>2.6249999999999999E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" s="12">
+        <v>2.6259999999999999E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>3.9539999999999999E-2</v>
       </c>
@@ -3886,11 +4019,14 @@
       <c r="D44" s="1">
         <v>3.9579999999999997E-2</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E44" s="12">
         <v>3.9609999999999999E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" s="12">
+        <v>3.9609999999999999E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <f>SUM(A4:A44)</f>
         <v>0.99999999999999978</v>
@@ -3899,8 +4035,44 @@
         <f>SUM(B4:B44)</f>
         <v>1.0000100000000001</v>
       </c>
+      <c r="C46" s="1">
+        <f t="shared" ref="C46:F46" si="0">SUM(C4:C44)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="D46" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0000200000000001</v>
+      </c>
+      <c r="E46" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0000099999999998</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0000199999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F48" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="13"/>
+    </row>
+    <row r="50" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="13"/>
+    </row>
+    <row r="51" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="13"/>
+    </row>
+    <row r="52" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E52" s="14"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F48:F51"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>